<commit_message>
mute ja ääni image ja inventoryn ase imageja
</commit_message>
<xml_diff>
--- a/documents/Sprintti 2 tehtävälista ja julkaisukäyrä, Java.xlsx
+++ b/documents/Sprintti 2 tehtävälista ja julkaisukäyrä, Java.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670"/>
   </bookViews>
   <sheets>
     <sheet name="Sprintin tehtävälista" sheetId="1" r:id="rId1"/>
@@ -724,11 +724,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63516032"/>
-        <c:axId val="63522304"/>
+        <c:axId val="142693888"/>
+        <c:axId val="142695808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63516032"/>
+        <c:axId val="142693888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,7 +757,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63522304"/>
+        <c:crossAx val="142695808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -765,7 +765,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63522304"/>
+        <c:axId val="142695808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,7 +795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63516032"/>
+        <c:crossAx val="142693888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1338,11 +1338,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1737,7 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="C4" s="15">
         <f ca="1">TODAY()</f>
-        <v>41367</v>
+        <v>41387</v>
       </c>
       <c r="D4" s="7"/>
       <c r="I4" s="2"/>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="D14" s="19" t="str">
         <f>'Sprintin tehtävälista'!G5</f>
-        <v>Ei vielä aloitettu</v>
+        <v>Kesken</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>